<commit_message>
added CB theme data
</commit_message>
<xml_diff>
--- a/movienames.xlsx
+++ b/movienames.xlsx
@@ -14,321 +14,636 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
-  <si>
-    <t>MOVIETITLES:American Beauty</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Cider House Rules</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Green Mile</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Insider</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Sixth Sense</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Gladiator</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Chocolat</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Crouching Tiger, Hidden Dragon</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Erin Brockovich</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Traffic</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:A Beautiful Mind</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Gosford Park</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:In the Bedroom</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Lord of the Rings: The Fellowship of the Ring</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Moulin Rouge!</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Chicago</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Gangs of New York</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Hours</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Lord of the Rings: The Two Towers</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Pianist</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Lord of the Rings: The Return of the King</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Lost in Translation</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Master and Commander: The Far Side of the World</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Mystic River</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Seabiscuit</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Million Dollar Baby</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Aviator</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Finding Neverland</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Ray</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Sideways</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Crash</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Brokeback Mountain</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Capote</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Good Night, and Good Luck.</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Munich</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Departed</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Babel</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Letters from Iwo Jima</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Little Miss Sunshine</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Queen</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:No Country for Old Men</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Atonement</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Juno</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Michael Clayton</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:There Will Be Blood</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Slumdog Millionaire</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Curious Case of Benjamin Button</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Frost/Nixon</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Milk</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Reader</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Hurt Locker</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:A Serious Man</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:An Education</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Avatar</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:District 9</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Inglourious Basterds</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Precious</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Blind Side</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Up</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Up in the Air</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The King's Speech</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:127 Hours</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Black Swan</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Fighter</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Inception</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Kids Are All Right</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Social Network</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Toy Story 3</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:True Grit</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Winter's Bone</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Artist</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Tree of Life</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Descendants</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Extremely Loud &amp; Incredibly Close</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Help</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Hugo</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Midnight in Paris</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Moneyball</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:War Horse</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Argo</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Amour</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Beasts of the Southern Wild</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Django Unchained</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Les Misérables</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Life of Pi</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Lincoln</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Silver Linings Playbook</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Zero Dark Thirty</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:12 Years a Slave</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Wolf of Wall Street</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:American Hustle</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Nebraska</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Captain Phillips</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Philomena</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Dallas Buyers Club</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Gravity</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Her</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Birdman or (The Unexpected Virtue of Ignorance)</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:American Sniper</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Boyhood</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Imitation Game</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Grand Budapest Hotel</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Selma</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:The Theory of Everything</t>
-  </si>
-  <si>
-    <t>MOVIETITLES:Whiplash</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
+  <si>
+    <t>MOVIETITLE:"American Beauty"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Cider House Rules"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Green Mile"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Insider"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Sixth Sense"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Gladiator"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Chocolat"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Crouching Tiger, Hidden Dragon"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Erin Brockovich"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Traffic"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"A Beautiful Mind"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Gosford Park"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"In the Bedroom"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Lord of the Rings: The Fellowship of the Ring"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Moulin Rouge!"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Chicago"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Gangs of New York"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Hours"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Lord of the Rings: The Two Towers"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Pianist"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Lord of the Rings: The Return of the King"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Lost in Translation"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Master and Commander: The Far Side of the World"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Mystic River"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Seabiscuit"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Million Dollar Baby"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Aviator"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Finding Neverland"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Ray"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Sideways"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Crash"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Brokeback Mountain"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Capote"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Good Night, and Good Luck."</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Munich"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Departed"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Babel"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Letters from Iwo Jima"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Little Miss Sunshine"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Queen"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"No Country for Old Men"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Atonement"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Juno"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Michael Clayton"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"There Will Be Blood"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Slumdog Millionaire"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Curious Case of Benjamin Button"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Frost/Nixon"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Milk"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Reader"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Hurt Locker"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"A Serious Man"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"An Education"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Avatar"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"District 9"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Inglourious Basterds"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Precious"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Blind Side"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Up"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Up in the Air"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The King's Speech"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"127 Hours"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Black Swan"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Fighter"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Inception"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Kids Are All Right"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Social Network"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Toy Story 3"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"True Grit"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Winter's Bone"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Artist"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Tree of Life"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Descendants"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Extremely Loud &amp; Incredibly Close"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Help"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Hugo"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Midnight in Paris"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Moneyball"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"War Horse"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Argo"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Amour"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Beasts of the Southern Wild"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Django Unchained"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Les Misérables"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Life of Pi"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Lincoln"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Silver Linings Playbook"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Zero Dark Thirty"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"12 Years a Slave"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Wolf of Wall Street"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"American Hustle"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Nebraska"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Captain Phillips"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Philomena"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Dallas Buyers Club"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Gravity"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Her"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Birdman or (The Unexpected Virtue of Ignorance)"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"American Sniper"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Boyhood"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Imitation Game"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Grand Budapest Hotel"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Selma"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"The Theory of Everything"</t>
+  </si>
+  <si>
+    <t>MOVIETITLE:"Whiplash"</t>
+  </si>
+  <si>
+    <t>American Beauty</t>
+  </si>
+  <si>
+    <t>The Cider House Rules</t>
+  </si>
+  <si>
+    <t>The Green Mile</t>
+  </si>
+  <si>
+    <t>The Insider</t>
+  </si>
+  <si>
+    <t>The Sixth Sense</t>
+  </si>
+  <si>
+    <t>Gladiator</t>
+  </si>
+  <si>
+    <t>Chocolat</t>
+  </si>
+  <si>
+    <t>Crouching Tiger, Hidden Dragon</t>
+  </si>
+  <si>
+    <t>Erin Brockovich</t>
+  </si>
+  <si>
+    <t>Traffic</t>
+  </si>
+  <si>
+    <t>A Beautiful Mind</t>
+  </si>
+  <si>
+    <t>Gosford Park</t>
+  </si>
+  <si>
+    <t>In the Bedroom</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings: The Fellowship of the Ring</t>
+  </si>
+  <si>
+    <t>Moulin Rouge!</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Gangs of New York</t>
+  </si>
+  <si>
+    <t>The Hours</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings: The Two Towers</t>
+  </si>
+  <si>
+    <t>The Pianist</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings: The Return of the King</t>
+  </si>
+  <si>
+    <t>Lost in Translation</t>
+  </si>
+  <si>
+    <t>Master and Commander: The Far Side of the World</t>
+  </si>
+  <si>
+    <t>Mystic River</t>
+  </si>
+  <si>
+    <t>Seabiscuit</t>
+  </si>
+  <si>
+    <t>Million Dollar Baby</t>
+  </si>
+  <si>
+    <t>The Aviator</t>
+  </si>
+  <si>
+    <t>Finding Neverland</t>
+  </si>
+  <si>
+    <t>Ray</t>
+  </si>
+  <si>
+    <t>Sideways</t>
+  </si>
+  <si>
+    <t>Crash</t>
+  </si>
+  <si>
+    <t>Brokeback Mountain</t>
+  </si>
+  <si>
+    <t>Capote</t>
+  </si>
+  <si>
+    <t>Good Night, and Good Luck.</t>
+  </si>
+  <si>
+    <t>Munich</t>
+  </si>
+  <si>
+    <t>The Departed</t>
+  </si>
+  <si>
+    <t>Babel</t>
+  </si>
+  <si>
+    <t>Letters from Iwo Jima</t>
+  </si>
+  <si>
+    <t>Little Miss Sunshine</t>
+  </si>
+  <si>
+    <t>The Queen</t>
+  </si>
+  <si>
+    <t>No Country for Old Men</t>
+  </si>
+  <si>
+    <t>Atonement</t>
+  </si>
+  <si>
+    <t>Juno</t>
+  </si>
+  <si>
+    <t>Michael Clayton</t>
+  </si>
+  <si>
+    <t>There Will Be Blood</t>
+  </si>
+  <si>
+    <t>Slumdog Millionaire</t>
+  </si>
+  <si>
+    <t>The Curious Case of Benjamin Button</t>
+  </si>
+  <si>
+    <t>Frost/Nixon</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>The Reader</t>
+  </si>
+  <si>
+    <t>The Hurt Locker</t>
+  </si>
+  <si>
+    <t>A Serious Man</t>
+  </si>
+  <si>
+    <t>An Education</t>
+  </si>
+  <si>
+    <t>Avatar</t>
+  </si>
+  <si>
+    <t>District 9</t>
+  </si>
+  <si>
+    <t>Inglourious Basterds</t>
+  </si>
+  <si>
+    <t>Precious</t>
+  </si>
+  <si>
+    <t>The Blind Side</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Up in the Air</t>
+  </si>
+  <si>
+    <t>The King's Speech</t>
+  </si>
+  <si>
+    <t>127 Hours</t>
+  </si>
+  <si>
+    <t>Black Swan</t>
+  </si>
+  <si>
+    <t>The Fighter</t>
+  </si>
+  <si>
+    <t>Inception</t>
+  </si>
+  <si>
+    <t>The Kids Are All Right</t>
+  </si>
+  <si>
+    <t>The Social Network</t>
+  </si>
+  <si>
+    <t>Toy Story 3</t>
+  </si>
+  <si>
+    <t>True Grit</t>
+  </si>
+  <si>
+    <t>Winter's Bone</t>
+  </si>
+  <si>
+    <t>The Artist</t>
+  </si>
+  <si>
+    <t>The Tree of Life</t>
+  </si>
+  <si>
+    <t>The Descendants</t>
+  </si>
+  <si>
+    <t>Extremely Loud &amp; Incredibly Close</t>
+  </si>
+  <si>
+    <t>The Help</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Midnight in Paris</t>
+  </si>
+  <si>
+    <t>Moneyball</t>
+  </si>
+  <si>
+    <t>War Horse</t>
+  </si>
+  <si>
+    <t>Argo</t>
+  </si>
+  <si>
+    <t>Amour</t>
+  </si>
+  <si>
+    <t>Beasts of the Southern Wild</t>
+  </si>
+  <si>
+    <t>Django Unchained</t>
+  </si>
+  <si>
+    <t>Les Misérables</t>
+  </si>
+  <si>
+    <t>Life of Pi</t>
+  </si>
+  <si>
+    <t>Lincoln</t>
+  </si>
+  <si>
+    <t>Silver Linings Playbook</t>
+  </si>
+  <si>
+    <t>Zero Dark Thirty</t>
+  </si>
+  <si>
+    <t>12 Years a Slave</t>
+  </si>
+  <si>
+    <t>The Wolf of Wall Street</t>
+  </si>
+  <si>
+    <t>American Hustle</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Captain Phillips</t>
+  </si>
+  <si>
+    <t>Philomena</t>
+  </si>
+  <si>
+    <t>Dallas Buyers Club</t>
+  </si>
+  <si>
+    <t>Gravity</t>
+  </si>
+  <si>
+    <t>Her</t>
+  </si>
+  <si>
+    <t>Birdman or (The Unexpected Virtue of Ignorance)</t>
+  </si>
+  <si>
+    <t>American Sniper</t>
+  </si>
+  <si>
+    <t>Boyhood</t>
+  </si>
+  <si>
+    <t>The Imitation Game</t>
+  </si>
+  <si>
+    <t>The Grand Budapest Hotel</t>
+  </si>
+  <si>
+    <t>Selma</t>
+  </si>
+  <si>
+    <t>The Theory of Everything</t>
+  </si>
+  <si>
+    <t>Whiplash</t>
   </si>
 </sst>
 </file>
@@ -686,855 +1001,1173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B106"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="B1" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="C62" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="C63" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="C64" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="C65" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="C66" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="C67" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="C68" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="C69" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="C70" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="C71" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="C72" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="C73" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="C74" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="C75" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="C76" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="C77" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="C78" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="C79" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="C80" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="C81" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="C82" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="C83" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="C84" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="C85" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="C86" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="C87" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="C88" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="C89" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="C90" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="C91" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="C92" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="C93" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:2">
+      <c r="C94" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="C95" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="C96" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="C97" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="C98" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="C99" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
+      <c r="C100" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="1:2">
+      <c r="C101" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" s="1">
         <v>100</v>
       </c>
       <c r="B102" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="103" spans="1:2">
+      <c r="C102" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" s="1">
         <v>101</v>
       </c>
       <c r="B103" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="104" spans="1:2">
+      <c r="C103" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" s="1">
         <v>102</v>
       </c>
       <c r="B104" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="C104" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" s="1">
         <v>103</v>
       </c>
       <c r="B105" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
+      <c r="C105" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" s="1">
         <v>104</v>
       </c>
       <c r="B106" t="s">
         <v>104</v>
+      </c>
+      <c r="C106" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>